<commit_message>
fix center .below-section in <md
</commit_message>
<xml_diff>
--- a/Phan-chia-viec.xlsx
+++ b/Phan-chia-viec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Front-End\cybersoft\BC35E_Capstone_HTML-CSS_Group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8529C616-D4F1-4517-A805-833F4DAEC3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5A8DF-7BD6-4124-9F05-694962E56FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{0DD9DC6C-51BF-4C5F-A98F-A4B5BF7049E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0DD9DC6C-51BF-4C5F-A98F-A4B5BF7049E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t xml:space="preserve">Section </t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>24/08</t>
+  </si>
+  <si>
+    <t>25/08</t>
   </si>
 </sst>
 </file>
@@ -663,10 +666,16 @@
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">

</xml_diff>

<commit_message>
toggle theme [1] [only change background of body]
</commit_message>
<xml_diff>
--- a/Phan-chia-viec.xlsx
+++ b/Phan-chia-viec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Front-End\cybersoft\BC35E_Capstone_HTML-CSS_Group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5A8DF-7BD6-4124-9F05-694962E56FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0D35B6-C20A-4FE8-9BD4-2959AF8F7626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0DD9DC6C-51BF-4C5F-A98F-A4B5BF7049E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t xml:space="preserve">Section </t>
   </si>
@@ -85,9 +85,6 @@
     <t>btn-backToTop</t>
   </si>
   <si>
-    <t>bar</t>
-  </si>
-  <si>
     <t>Thời gian BĐ</t>
   </si>
   <si>
@@ -116,6 +113,12 @@
   </si>
   <si>
     <t>25/08</t>
+  </si>
+  <si>
+    <t>toggle theme</t>
+  </si>
+  <si>
+    <t>26/08</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,10 +518,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -532,14 +535,14 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -547,14 +550,14 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -562,14 +565,14 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -577,14 +580,14 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -592,14 +595,14 @@
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -607,14 +610,14 @@
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -667,14 +670,14 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -682,24 +685,30 @@
         <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>